<commit_message>
add heatmap view and scatter point map view
</commit_message>
<xml_diff>
--- a/address.xlsx
+++ b/address.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="5">
   <si>
     <t>address</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -23,22 +23,20 @@
     <t>四川省自贡市自流井区高笋塘小区17栋1单元28号</t>
   </si>
   <si>
-    <t>四川省自贡市自流井区鸿鹤路43号</t>
+    <t>四川省荣县旭阳镇望佛街6号4栋2单元202号</t>
   </si>
   <si>
-    <t>四川省自贡市汇东新区银桦小区9组14栋1单元6楼</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>四川省自贡市自流井区中昊黑元化工研究设计院有限公司</t>
   </si>
   <si>
-    <t>四川省自贡市自流井区西林街169号 </t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>四川省自贡市自流井区丹桂大街541号</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -52,12 +50,6 @@
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF032F62"/>
-      <name val="Consolas"/>
-      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -82,7 +74,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -392,7 +384,7 @@
   <dimension ref="A1:A15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A13" sqref="A13:A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -412,60 +404,68 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>